<commit_message>
new data for paper
</commit_message>
<xml_diff>
--- a/experimental_data_collection/kmeans/validation_data.xlsx
+++ b/experimental_data_collection/kmeans/validation_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ceccarelli/Google Drive/REU/REU-Drone-Swarm-Optimization/experimental_data_collection/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ceccarelli/Google Drive/REU/REU-Drone-Swarm-Optimization/experimental_data_collection/kmeans/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{640BD69E-75DC-FA45-9F0B-B3ECFC45FAC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D706A90A-CCD7-8E4C-80C4-34EB05B6B567}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{78AB08D8-FB54-DB4B-828C-07D50BFD4035}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" xr2:uid="{78AB08D8-FB54-DB4B-828C-07D50BFD4035}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -333,12 +333,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Optimal</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Solution Success vs Number of User Clusters</a:t>
+              <a:t>Solution Success vs Number of User Clusters</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2457,16 +2453,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>311150</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>425450</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>755650</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2501,8 +2497,8 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2829,8 +2825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1F986A9-5491-D247-B935-12EFEC76C144}">
   <dimension ref="B2:BD46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="N51" sqref="N51"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="N64" sqref="N64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>